<commit_message>
[DOCS] typos : missing semicolon and useless operators factorisation
</commit_message>
<xml_diff>
--- a/docs/grammar/(step3)grammar_without_left_rec.xlsx
+++ b/docs/grammar/(step3)grammar_without_left_rec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanmzx/Developer/mezureux1u/docs/grammar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CF1A02-191C-FB4F-A5CC-867126AAF48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6DCA6A-1EEC-4F45-B133-4863E34497D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3560" yWindow="-20640" windowWidth="37520" windowHeight="20160" xr2:uid="{9D692640-1C59-1F40-B61E-C86534EBD592}"/>
   </bookViews>
@@ -474,9 +474,6 @@
     <t>caractere EXPR_REC</t>
   </si>
   <si>
-    <t>with Ada.Text_IO use Ada.Text_IO; PROCEDURE BEGIN_INSTR ; EOF</t>
-  </si>
-  <si>
     <t>with Ada ". "Text"_"IO use Ada "." Text"_"IO";" PROCEDURE BEGIN_INSTR ";" EOF</t>
   </si>
   <si>
@@ -532,6 +529,9 @@
   </si>
   <si>
     <t>type ident is record CHAMPS end record ";"</t>
+  </si>
+  <si>
+    <t>with Ada.Text_IO ; use Ada.Text_IO; PROCEDURE BEGIN_INSTR ; EOF</t>
   </si>
 </sst>
 </file>
@@ -913,7 +913,7 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,7 +932,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>107</v>
@@ -2266,7 +2266,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>107</v>
@@ -2280,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>107</v>
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>107</v>
@@ -2770,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>107</v>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>107</v>
@@ -2880,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>107</v>
@@ -2950,7 +2950,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>107</v>
@@ -2964,7 +2964,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>107</v>
@@ -3020,7 +3020,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>107</v>
@@ -3188,7 +3188,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>107</v>
@@ -3202,7 +3202,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>107</v>
@@ -3230,7 +3230,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>107</v>
@@ -3244,7 +3244,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>107</v>
@@ -3258,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>107</v>
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>107</v>
@@ -3286,7 +3286,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>107</v>
@@ -3300,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>107</v>
@@ -3314,7 +3314,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>107</v>

</xml_diff>